<commit_message>
Update ML to v0.2 - implement categorical to MLR
</commit_message>
<xml_diff>
--- a/docs/examples and guides/input data/Data.xlsx
+++ b/docs/examples and guides/input data/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\docs\examples and guides\input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621E2BA7-6E04-474A-97FB-9E58A90CE670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70CEEA9-DA9F-4A04-86DE-EBCBFB3C4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
     <sheet name="Design Parameters" sheetId="1" r:id="rId3"/>
     <sheet name="Responses" sheetId="3" r:id="rId4"/>
+    <sheet name="Misc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -100,7 +101,7 @@
     Each row is the name of each feature. Should match the feature names in the “Data” sheet </t>
       </text>
     </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +109,7 @@
     The minimum level of this feature.</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +117,7 @@
     The maximum level of this feature.</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -162,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Features</t>
   </si>
@@ -213,6 +214,15 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Feature type</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
   <si>
     <t>-2,-1,-0.5,0,0.5,1,2</t>
@@ -643,13 +653,13 @@
   <threadedComment ref="B1" dT="2024-07-09T18:31:44.34" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BC7AD3A8-5E18-4A5C-9728-B3CD7668C3E2}">
     <text xml:space="preserve">Each row is the name of each feature. Should match the feature names in the “Data” sheet </text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2024-07-09T18:32:18.60" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
+  <threadedComment ref="D1" dT="2024-07-09T18:32:18.60" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
     <text>The minimum level of this feature.</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2024-07-09T18:32:26.48" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
+  <threadedComment ref="E1" dT="2024-07-09T18:32:26.48" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
     <text>The maximum level of this feature.</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2024-07-09T18:33:05.39" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
+  <threadedComment ref="F1" dT="2024-07-09T18:33:05.39" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
     <text>Dropdown, denotes whether the feature is a Mixture or Process feature. When in doubt, set to Process.</text>
   </threadedComment>
 </ThreadedComments>
@@ -676,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7017105-9951-4AAA-B498-721790E5798E}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1168,22 +1178,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A90CAD-67BE-406A-8BD7-81EDC587CCAA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="40.90625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1191,70 +1202,85 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1">
         <v>85</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>145</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
         <v>2.7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>3.2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
         <v>28</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{E365AB81-AF3B-4DDA-A9DD-340913AC677F}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{E365AB81-AF3B-4DDA-A9DD-340913AC677F}">
       <formula1>"Process,Mixture"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{A24BB7C6-2CFF-4AC1-A2A1-DC71321121EE}">
+      <formula1>"Numerical, Categorical"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1267,7 +1293,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1290,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,11 +1324,34 @@
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996A7378-54BB-494D-84D1-CDC0B6ABA572}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>